<commit_message>
Updates to prepare for upload.
</commit_message>
<xml_diff>
--- a/Planning and Design/SprintBurnDown_Sprint_1.xlsx
+++ b/Planning and Design/SprintBurnDown_Sprint_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\source\CST-323\CST-247-Project\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DE4D41-4C2F-4FEF-8A3D-327548F02803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA306F92-5A4A-4154-B800-68A2FB5E7628}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2798" yWindow="1763" windowWidth="20490" windowHeight="13094" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="712" windowWidth="20490" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -94,15 +94,6 @@
     <t>Task 3</t>
   </si>
   <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
     <t>User Story</t>
   </si>
   <si>
@@ -160,51 +151,36 @@
     <t>After each Daily Standup each Team Member should review the Burn Down Chart to ensure your Sprint will be delivered on time</t>
   </si>
   <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>Richard</t>
+  </si>
+  <si>
     <t>Project Title: Minesweeper
-Release #: 1.0
+Release #: 0
 Sprint #: 1</t>
   </si>
   <si>
-    <t>M2-1</t>
-  </si>
-  <si>
-    <t>M2-2</t>
-  </si>
-  <si>
-    <t>M2-3</t>
-  </si>
-  <si>
-    <t>M2-4</t>
-  </si>
-  <si>
-    <t>M2-6</t>
-  </si>
-  <si>
-    <t>M2-5</t>
-  </si>
-  <si>
-    <t>I would like to setup the database so we can save data</t>
-  </si>
-  <si>
-    <t>I would like to create login and registration controllers</t>
-  </si>
-  <si>
-    <t>I would like to create models for user and registration</t>
-  </si>
-  <si>
-    <t>I would like to create views that are consumed by controllers</t>
-  </si>
-  <si>
-    <t>I would like to insure that controllers and views validate data</t>
-  </si>
-  <si>
-    <t>I would like to update design documentation</t>
-  </si>
-  <si>
-    <t>Shawn</t>
-  </si>
-  <si>
-    <t>Richard</t>
+    <t>M1-1</t>
+  </si>
+  <si>
+    <t>M1-2</t>
+  </si>
+  <si>
+    <t>M1-3</t>
+  </si>
+  <si>
+    <t>Plan our release using agile format so that we can meet our deadline.</t>
+  </si>
+  <si>
+    <t>Create product backlog, sprint backlog and initial burndown so that we follow our plan set forth in release planning.</t>
+  </si>
+  <si>
+    <t>Create initial UI and Design Documentation so that we can plan the intial look of the application, communicate our plan and have a method of delivery to stake holders.</t>
+  </si>
+  <si>
+    <t>Richard and Shawn</t>
   </si>
 </sst>
 </file>
@@ -458,34 +434,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.1</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1999999999999993</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.2999999999999989</c:v>
+                  <c:v>2.8000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3999999999999986</c:v>
+                  <c:v>2.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4999999999999982</c:v>
+                  <c:v>2.0000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.5999999999999983</c:v>
+                  <c:v>1.6000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.6999999999999984</c:v>
+                  <c:v>1.2000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7999999999999985</c:v>
+                  <c:v>0.8000000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.89999999999999847</c:v>
+                  <c:v>0.40000000000000058</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.5543122344752192E-15</c:v>
+                  <c:v>5.5511151231257827E-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -566,19 +542,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -976,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -990,7 +966,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1025,7 +1001,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -1072,16 +1048,16 @@
     <row r="4" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4">
         <v>2</v>
@@ -1090,19 +1066,19 @@
         <v>0</v>
       </c>
       <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
         <v>2</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
       </c>
       <c r="M4" s="4">
         <v>0</v>
@@ -1119,19 +1095,19 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
@@ -1140,19 +1116,19 @@
         <v>0</v>
       </c>
       <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
         <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0</v>
       </c>
       <c r="M5" s="4">
         <v>0</v>
@@ -1169,19 +1145,19 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" ht="114" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -1193,16 +1169,16 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <v>1</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
@@ -1219,22 +1195,14 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="B7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -1252,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="4">
         <v>0</v>
@@ -1269,22 +1237,14 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
-      <c r="B8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -1302,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M8" s="4">
         <v>0</v>
@@ -1319,22 +1279,14 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
-      <c r="B9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -1352,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="4">
         <v>0</v>
@@ -1413,10 +1365,12 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="4">
         <v>0</v>
       </c>
@@ -1455,10 +1409,12 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="4">
         <v>0</v>
       </c>
@@ -1497,10 +1453,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="4">
         <v>0</v>
       </c>
@@ -1539,90 +1495,86 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
-      <c r="B14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="4">
         <f>SUM(F4:F13)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G14" s="4">
         <f>F14-$F$14/10</f>
-        <v>8.1</v>
+        <v>3.6</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14:P14" si="0">G14-$F$14/10</f>
-        <v>7.1999999999999993</v>
+        <v>3.2</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>6.2999999999999989</v>
+        <v>2.8000000000000003</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>5.3999999999999986</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>4.4999999999999982</v>
+        <v>2.0000000000000004</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>3.5999999999999983</v>
+        <v>1.6000000000000005</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="0"/>
-        <v>2.6999999999999984</v>
+        <v>1.2000000000000006</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="0"/>
-        <v>1.7999999999999985</v>
+        <v>0.8000000000000006</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" si="0"/>
-        <v>0.89999999999999847</v>
+        <v>0.40000000000000058</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" si="0"/>
-        <v>-1.5543122344752192E-15</v>
+        <v>5.5511151231257827E-16</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
-      <c r="B15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="4">
         <f>SUM(F4:F13)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" ref="G15:P15" si="1">F15 - SUM(G4:G13)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
@@ -2029,10 +1981,6 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2049,10 +1997,6 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2069,10 +2013,6 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2089,8 +2029,8 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2118,74 +2058,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">

</xml_diff>